<commit_message>
clean up and add individual plots
</commit_message>
<xml_diff>
--- a/Table_Processing/Filter_CD05_A.xlsx
+++ b/Table_Processing/Filter_CD05_A.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lea/ContrastiveDecodingNew/Table_Processing/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D23509-99D3-9448-A72A-5A210DB88ACD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3400" yWindow="500" windowWidth="32000" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter CD05 A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,10 +54,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -62,17 +76,23 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="plot_0.5_90.png"/>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>118545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="plot_0.5_90.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -85,8 +105,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10972822" cy="5486411"/>
+          <a:off x="0" y="152400"/>
+          <a:ext cx="12192022" cy="5367878"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>16955</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>50810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="plot_0.5_281.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16933" y="5503333"/>
+          <a:ext cx="12192022" cy="5350944"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -99,32 +163,38 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>135466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="plot_0.5_281.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3810000"/>
-          <a:ext cx="10972822" cy="5486411"/>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>84678</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="plot_0.5_490.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10752666"/>
+          <a:ext cx="12192022" cy="5350945"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -137,32 +207,82 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>169973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>21</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>128655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="plot_0.5_533.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16853155"/>
+          <a:ext cx="12053476" cy="5650591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="plot_0.5_490.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="7620000"/>
-          <a:ext cx="10972822" cy="5486411"/>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>177811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="plot_0.5_679.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22987000"/>
+          <a:ext cx="12344422" cy="5842011"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -175,32 +295,38 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="plot_0.5_533.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="11430000"/>
-          <a:ext cx="10972822" cy="5486411"/>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>101611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="plot_0.5_863.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28803600"/>
+          <a:ext cx="12344422" cy="5842011"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -213,32 +339,38 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>152411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="plot_0.5_679.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="15240000"/>
-          <a:ext cx="10972822" cy="5486411"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="plot_0.5_873.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="34544000"/>
+          <a:ext cx="12344422" cy="5842011"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -251,31 +383,81 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>22</xdr:colOff>
-      <xdr:row>128</xdr:row>
+      <xdr:row>226</xdr:row>
       <xdr:rowOff>152411</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="plot_0.5_863.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="19050000"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="plot_0.5_875.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="40233600"/>
+          <a:ext cx="12344422" cy="5842011"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>237056</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>372544</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>16945</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 1" descr="plot_0.9_90.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD939BC5-6A49-5E48-A589-B4075F94AB35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11074389" y="118534"/>
           <a:ext cx="10972822" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -287,109 +469,303 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>22</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="plot_0.5_873.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="22860000"/>
-          <a:ext cx="10972822" cy="5486411"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>140</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>22</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="plot_0.5_875.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="26670000"/>
-          <a:ext cx="10972822" cy="5486411"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>22</xdr:colOff>
-      <xdr:row>188</xdr:row>
-      <xdr:rowOff>152411</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="plot_0.5_Idx.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="30480000"/>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>262456</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>59267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>397944</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>143944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 2" descr="plot_0.9_281.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE9FB628-CA96-1B4F-A2A6-E62ACD3D649B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11235256" y="5952067"/>
+          <a:ext cx="11108288" cy="5977477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>262456</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>143933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>397944</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>42344</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 3" descr="plot_0.9_490.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8E9CAC-0D81-F444-8E8A-1FB0CE3BF8C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11235256" y="11726333"/>
+          <a:ext cx="11108288" cy="5994411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287856</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>423344</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>145483</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 4" descr="plot_0.9_533.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEF71F0-7A9D-D840-B6C0-D80B9FC9F9BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11002038" y="16947188"/>
+          <a:ext cx="10849670" cy="5769659"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287856</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>423344</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>177811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 5" descr="plot_0.9_679.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB63E86A-70D2-0B42-AA7D-77349256389D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11260656" y="23444200"/>
+          <a:ext cx="11108288" cy="5994411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>262456</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>397944</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>8478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 7" descr="plot_0.9_873.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8641E264-34C7-694D-9950-63A1D4FE9B68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11235256" y="34654067"/>
+          <a:ext cx="11108288" cy="5994411"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>242631</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>79092</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>378119</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>163769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 8" descr="plot_0.9_875.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8EDD45C-60AF-AE4F-AC3D-FE0625A50D2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11146046" y="36878116"/>
+          <a:ext cx="11038902" cy="5474433"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>330189</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>76195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>330211</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>76206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 6" descr="plot_0.9_863.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EF0CB45-97DA-024A-92C0-E2465A35D3ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11302989" y="29336995"/>
           <a:ext cx="10972822" cy="5486411"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -403,7 +779,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -445,7 +821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,9 +853,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,6 +905,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -686,12 +1098,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O235" sqref="O235"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>